<commit_message>
update export tab name to match csv file and var name
</commit_message>
<xml_diff>
--- a/InputData/trans/BNoGP/BAU Number of Gas Pumps.xlsx
+++ b/InputData/trans/BNoGP/BAU Number of Gas Pumps.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BNoGP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\United States\us-eps\InputData\trans\BNoGP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E3F452-B6BC-4F2A-B6ED-381F725D5387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079A797E-B4DD-42F9-A04A-A3DE945D70FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="795" yWindow="45" windowWidth="16110" windowHeight="8835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
-    <sheet name="BNoEVC" sheetId="3" r:id="rId2"/>
+    <sheet name="BNoGP" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="income">#REF!</definedName>
@@ -66,10 +66,10 @@
     <t>BAU EV Chargers</t>
   </si>
   <si>
-    <t>BNoEVC BAU Number of EV Chargers</t>
-  </si>
-  <si>
     <t>We assume the number of gas pumps remains relatively constant.</t>
+  </si>
+  <si>
+    <t>BNoEVC BAU Number of Gas Pumps</t>
   </si>
 </sst>
 </file>
@@ -421,8 +421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,7 +433,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -471,7 +471,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -487,8 +487,8 @@
   </sheetPr>
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AE2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
[trans/BNoGP] update "BAU EV Chargers" text to "BAU Gas Pumps"
</commit_message>
<xml_diff>
--- a/InputData/trans/BNoGP/BAU Number of Gas Pumps.xlsx
+++ b/InputData/trans/BNoGP/BAU Number of Gas Pumps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\United States\us-eps\InputData\trans\BNoGP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Desktop\Dropbox_Free_Zone\EPS\Model Repos\eps-us\InputData\trans\BNoGP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079A797E-B4DD-42F9-A04A-A3DE945D70FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1B5AEA-3A11-463F-9E0D-2C706DCF7B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="795" yWindow="45" windowWidth="16110" windowHeight="8835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="555" yWindow="885" windowWidth="22950" windowHeight="13650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -63,13 +63,13 @@
     <t>Number of chargers</t>
   </si>
   <si>
-    <t>BAU EV Chargers</t>
-  </si>
-  <si>
     <t>We assume the number of gas pumps remains relatively constant.</t>
   </si>
   <si>
     <t>BNoEVC BAU Number of Gas Pumps</t>
+  </si>
+  <si>
+    <t>BAU Gas Pumps</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -471,7 +471,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -487,9 +487,7 @@
   </sheetPr>
   <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -593,7 +591,7 @@
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2">
         <v>1200000</v>

</xml_diff>